<commit_message>
Added United Way data
</commit_message>
<xml_diff>
--- a/Non-Profit Organization Data/Data Collection.xlsx
+++ b/Non-Profit Organization Data/Data Collection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffb294a4d76353ad/Documents/SRVC/Git/Non-Profit Organization Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\party\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7175C40F-D922-456D-84F2-06144233E1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F91B5EC-628A-4DEB-9691-907B44A60232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0F9B7CC6-A737-449A-8710-FBCC55CAE590}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Title of Organization</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>United Way of San Luis Obispo</t>
+  </si>
+  <si>
+    <t>35.279577</t>
+  </si>
+  <si>
+    <t>-120.660200</t>
+  </si>
+  <si>
+    <t>To foster structural change by addressing root causes in order to safeguard the future of our community.</t>
+  </si>
+  <si>
+    <t>https://www.unitedwayslo.org/about-us</t>
+  </si>
+  <si>
+    <t>https://www.unitedwayslo.org</t>
+  </si>
+  <si>
+    <t>https://www.volunteerslo.org/need/index?q=united+way</t>
   </si>
 </sst>
 </file>
@@ -143,11 +164,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -157,11 +175,20 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -478,62 +505,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9556E4BF-6520-4213-BCFA-5ABDE17D5B86}">
-  <dimension ref="B1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" style="9" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.85546875" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="8">
@@ -543,84 +572,98 @@
         <v>-120.66750500000001</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
+    <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
@@ -630,8 +673,14 @@
     <hyperlink ref="E3" r:id="rId1" xr:uid="{51DCD241-FCA0-4CD0-8A60-03ABE1DD5C1C}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{BCEE4BF9-D2A2-422A-8471-C99E4180AE7E}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{D34995AE-E493-41A9-B3C9-072AAF23945A}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{D0F39F50-CFAF-4B24-A4D8-0D5D11789A5A}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{8C65FE82-CEC2-4756-AD17-D6744DFBBDB3}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{BBAEA6B6-83EF-430C-BF51-8A9E6F3AF329}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
+  <ignoredErrors>
+    <ignoredError sqref="G4" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>